<commit_message>
Added solubility curve for NRTL
</commit_message>
<xml_diff>
--- a/examples/Database/Tulashie_Parameters.xlsx
+++ b/examples/Database/Tulashie_Parameters.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rgp11/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rgp11/.julia/dev/SolMod/examples/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B92797A-CACC-3B49-AA45-EEA5C4546261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBF585C-86B2-A441-BCB5-B586AA0C2CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13980" activeTab="2" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="11080" yWindow="0" windowWidth="14520" windowHeight="16000" activeTab="1" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Solute" sheetId="1" r:id="rId1"/>
-    <sheet name="Ethyl Lactate" sheetId="8" r:id="rId2"/>
-    <sheet name="Diethyl Tartrate" sheetId="9" r:id="rId3"/>
+    <sheet name="Diethyl Tartrate" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>fusΔH</t>
   </si>
@@ -460,11 +459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F0752-A0DB-C54D-AE19-41566BE58CC1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C286A7E9-06CA-244C-8AEB-FC3234EDBEEC}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,101 +493,6 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.9407999999999999E-3</v>
-      </c>
-      <c r="C2">
-        <v>0.57533000000000001</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>106910</v>
-      </c>
-      <c r="F2">
-        <v>31028</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1.9407999999999999E-3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0.57533000000000001</v>
-      </c>
-      <c r="D3">
-        <v>-100420</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>31028</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0.57533000000000001</v>
-      </c>
-      <c r="B4">
-        <v>0.57533000000000001</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>-2.9342000000000001</v>
-      </c>
-      <c r="E4">
-        <v>-2.9342000000000001</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C286A7E9-06CA-244C-8AEB-FC3234EDBEEC}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
         <v>0.97974799999999995</v>
       </c>
       <c r="C2">

</xml_diff>